<commit_message>
pump current calculation added, lambda calculation added, some change
</commit_message>
<xml_diff>
--- a/software/berechnungen.xlsx
+++ b/software/berechnungen.xlsx
@@ -1,20 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{381E4EEA-E3B6-4BE7-811E-33D336E78B84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="705" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="10035" yWindow="1740" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="ADC" sheetId="1" r:id="rId1"/>
+    <sheet name="Ip" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>ADC Referenz, V</t>
   </si>
@@ -29,12 +41,33 @@
   </si>
   <si>
     <t>Volt zu ADC</t>
+  </si>
+  <si>
+    <t>Ua</t>
+  </si>
+  <si>
+    <t>Ua_cal</t>
+  </si>
+  <si>
+    <t>Diff</t>
+  </si>
+  <si>
+    <t>amp</t>
+  </si>
+  <si>
+    <t>Rshunt</t>
+  </si>
+  <si>
+    <t>Ip</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -64,8 +97,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -84,7 +118,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -159,6 +193,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -194,6 +245,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -369,10 +437,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
@@ -433,4 +501,91 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64170B6A-AD63-4770-9569-9EDA834974F5}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1">
+        <v>0.51</v>
+      </c>
+      <c r="C1">
+        <f>B1*1000</f>
+        <v>510</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1.5</v>
+      </c>
+      <c r="C2">
+        <f>B2*1000</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <f>B1-B2</f>
+        <v>-0.99</v>
+      </c>
+      <c r="C3">
+        <f>C1-C2</f>
+        <v>-990</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>61.9</v>
+      </c>
+      <c r="C5">
+        <v>61.9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1">
+        <f>((B1-B2)/(B4*B5))*1000</f>
+        <v>-1.9991922455573503</v>
+      </c>
+      <c r="C7">
+        <f>(C1-C2)/(C4*C5)</f>
+        <v>-1.9991922455573505</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>